<commit_message>
changes in view.py file
</commit_message>
<xml_diff>
--- a/Final_File/Main_Portfolio_Momentum_Ranking.xlsx
+++ b/Final_File/Main_Portfolio_Momentum_Ranking.xlsx
@@ -594,79 +594,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.8974637158227678</c:v>
+                  <c:v>0.8974503214619483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7515903722702155</c:v>
+                  <c:v>0.7515949802543345</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66316073431648</c:v>
+                  <c:v>0.6631894861321259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.550428181377655</c:v>
+                  <c:v>0.5504359545535373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5204715599289735</c:v>
+                  <c:v>0.5205144937098669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2757818961868428</c:v>
+                  <c:v>0.276580293293589</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1837916383460498</c:v>
+                  <c:v>0.1838274393408871</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1594744287757374</c:v>
+                  <c:v>0.1594954086215743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1083667896113327</c:v>
+                  <c:v>0.1083958709210499</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.07094685194704484</c:v>
+                  <c:v>0.0709909194412266</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.08211668241687736</c:v>
+                  <c:v>-0.08207068385290703</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.1518764706388896</c:v>
+                  <c:v>-0.1518376363687866</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.1570068073199438</c:v>
+                  <c:v>-0.1569486519214684</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.2833517186992346</c:v>
+                  <c:v>-0.2833105233915634</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.3242812299442913</c:v>
+                  <c:v>-0.3242303930706905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.3279316253574075</c:v>
+                  <c:v>-0.3278629038008067</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.3804906461266385</c:v>
+                  <c:v>-0.380446218798042</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.4369978687334783</c:v>
+                  <c:v>-0.4369501105656562</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.4378988819948866</c:v>
+                  <c:v>-0.4378371307850757</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.4577823386510476</c:v>
+                  <c:v>-0.457736268279459</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.4818427872770104</c:v>
+                  <c:v>-0.4817842688840067</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.4999355241466834</c:v>
+                  <c:v>-0.4998914593316877</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.5101803069995212</c:v>
+                  <c:v>-0.5101424020616599</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.5869378541529165</c:v>
+                  <c:v>-0.5868696886135535</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.6245127507780308</c:v>
+                  <c:v>-0.6244536751828806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -882,79 +882,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-1.166427184952775</c:v>
+                  <c:v>-1.166358310563044</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.002563825653158</c:v>
+                  <c:v>-1.00249238272522</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.981937729118471</c:v>
+                  <c:v>-0.981867085582515</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.9580990199963619</c:v>
+                  <c:v>-0.9606878928251266</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.8603466780777715</c:v>
+                  <c:v>-0.8602937545102809</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.849597873141724</c:v>
+                  <c:v>-0.8495392040495664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.8400401577067147</c:v>
+                  <c:v>-0.8399806034064605</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.8344280319534016</c:v>
+                  <c:v>-0.8343724330688174</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.7966299655373175</c:v>
+                  <c:v>-0.7965682140893748</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.7666595037493592</c:v>
+                  <c:v>-0.7665867558991445</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.7536893927457834</c:v>
+                  <c:v>-0.7536279135873847</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.6245127507780308</c:v>
+                  <c:v>-0.6244536751828806</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.5869378541529165</c:v>
+                  <c:v>-0.5868696886135535</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.5101803069995212</c:v>
+                  <c:v>-0.5101424020616599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.4999355241466834</c:v>
+                  <c:v>-0.4998914593316877</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.4818427872770104</c:v>
+                  <c:v>-0.4817842688840067</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.4577823386510476</c:v>
+                  <c:v>-0.457736268279459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.4378988819948866</c:v>
+                  <c:v>-0.4378371307850757</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.4369978687334783</c:v>
+                  <c:v>-0.4369501105656562</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.3804906461266385</c:v>
+                  <c:v>-0.380446218798042</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.3279316253574075</c:v>
+                  <c:v>-0.3278629038008067</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.3242812299442913</c:v>
+                  <c:v>-0.3242303930706905</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.2833517186992346</c:v>
+                  <c:v>-0.2833105233915634</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.1570068073199438</c:v>
+                  <c:v>-0.1569486519214684</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.1518764706388896</c:v>
+                  <c:v>-0.1518376363687866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,16 +1541,16 @@
         <v>0.01152200000000003</v>
       </c>
       <c r="K4" s="3">
-        <v>1.251859954839093</v>
+        <v>1.252020141799833</v>
       </c>
       <c r="L4" s="3">
-        <v>3.23751852279332</v>
+        <v>3.237246351851301</v>
       </c>
       <c r="M4" s="3">
-        <v>0.3444478166354552</v>
+        <v>0.3445111682097665</v>
       </c>
       <c r="N4" s="3">
-        <v>-0.347802328541365</v>
+        <v>-0.3477570742294109</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -1586,13 +1586,13 @@
         <v>36</v>
       </c>
       <c r="Z4" s="3">
-        <v>1.022463715822768</v>
+        <v>1.022450321461948</v>
       </c>
       <c r="AA4">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB4" s="3">
-        <v>0.8974637158227678</v>
+        <v>0.8974503214619483</v>
       </c>
       <c r="AC4">
         <v>1</v>
@@ -1627,16 +1627,16 @@
         <v>0.04519641354342707</v>
       </c>
       <c r="K5" s="3">
-        <v>-1.482246573316043</v>
+        <v>-1.481991294163881</v>
       </c>
       <c r="L5" s="3">
-        <v>1.296806047459171</v>
+        <v>1.296713098929854</v>
       </c>
       <c r="M5" s="3">
-        <v>2.544420525329981</v>
+        <v>2.544507869236216</v>
       </c>
       <c r="N5" s="3">
-        <v>2.116027700810766</v>
+        <v>2.115953928765592</v>
       </c>
       <c r="O5">
         <v>-2</v>
@@ -1672,13 +1672,13 @@
         <v>37</v>
       </c>
       <c r="Z5" s="3">
-        <v>1.001590372270216</v>
+        <v>1.001594980254334</v>
       </c>
       <c r="AA5">
         <v>-0.9999999999999998</v>
       </c>
       <c r="AB5" s="3">
-        <v>0.7515903722702155</v>
+        <v>0.7515949802543345</v>
       </c>
       <c r="AC5">
         <v>2</v>
@@ -1713,16 +1713,16 @@
         <v>0.007770999999999972</v>
       </c>
       <c r="K6" s="3">
-        <v>4.166882026735045</v>
+        <v>4.166940829263979</v>
       </c>
       <c r="L6" s="3">
-        <v>0.9288769415444466</v>
+        <v>0.9288179708160164</v>
       </c>
       <c r="M6" s="3">
-        <v>0.1817704713459624</v>
+        <v>0.181832048803327</v>
       </c>
       <c r="N6" s="3">
-        <v>-0.622248873191106</v>
+        <v>-0.6221903605082224</v>
       </c>
       <c r="O6">
         <v>3</v>
@@ -1758,13 +1758,13 @@
         <v>36</v>
       </c>
       <c r="Z6" s="3">
-        <v>0.7881607343164799</v>
+        <v>0.7881894861321258</v>
       </c>
       <c r="AA6">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB6" s="3">
-        <v>0.66316073431648</v>
+        <v>0.6631894861321259</v>
       </c>
       <c r="AC6">
         <v>3</v>
@@ -1799,16 +1799,16 @@
         <v>0.05321653603768906</v>
       </c>
       <c r="K7" s="3">
-        <v>-0.7088733705681374</v>
+        <v>-0.7086449893264553</v>
       </c>
       <c r="L7" s="3">
-        <v>0.4428471349657365</v>
+        <v>0.4428330484927987</v>
       </c>
       <c r="M7" s="3">
-        <v>1.07952337253551</v>
+        <v>1.079594740653234</v>
       </c>
       <c r="N7" s="3">
-        <v>2.702829861892565</v>
+        <v>2.702727741737839</v>
       </c>
       <c r="O7">
         <v>-2</v>
@@ -1844,13 +1844,13 @@
         <v>37</v>
       </c>
       <c r="Z7" s="3">
-        <v>0.800428181377655</v>
+        <v>0.8004359545535373</v>
       </c>
       <c r="AA7">
         <v>-0.9999999999999998</v>
       </c>
       <c r="AB7" s="3">
-        <v>0.550428181377655</v>
+        <v>0.5504359545535373</v>
       </c>
       <c r="AC7">
         <v>4</v>
@@ -1885,16 +1885,16 @@
         <v>0.0164979999999999</v>
       </c>
       <c r="K8" s="3">
-        <v>1.555830665718934</v>
+        <v>1.555980280582088</v>
       </c>
       <c r="L8" s="3">
-        <v>0.6332466619977388</v>
+        <v>0.633214992362408</v>
       </c>
       <c r="M8" s="3">
-        <v>0.8790257213683046</v>
+        <v>0.8790949029106326</v>
       </c>
       <c r="N8" s="3">
-        <v>0.01627285305742284</v>
+        <v>0.01630051908525421</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -1930,13 +1930,13 @@
         <v>36</v>
       </c>
       <c r="Z8" s="3">
-        <v>0.6454715599289735</v>
+        <v>0.6455144937098668</v>
       </c>
       <c r="AA8">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB8" s="3">
-        <v>0.5204715599289735</v>
+        <v>0.5205144937098669</v>
       </c>
       <c r="AC8">
         <v>5</v>
@@ -1950,37 +1950,37 @@
         <v>5</v>
       </c>
       <c r="D9" s="2">
-        <v>0.1019</v>
+        <v>0.1021</v>
       </c>
       <c r="E9" s="2">
-        <v>0.187</v>
+        <v>0.1872</v>
       </c>
       <c r="F9" s="2">
-        <v>0.005344</v>
+        <v>0.005347999999999999</v>
       </c>
       <c r="G9" s="2">
-        <v>0.036051</v>
+        <v>0.036061</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>0.005344000000000015</v>
+        <v>0.005347999999999908</v>
       </c>
       <c r="J9" s="2">
-        <v>0.03605100000000006</v>
+        <v>0.0360609999999999</v>
       </c>
       <c r="K9" s="3">
-        <v>0.7718633095087277</v>
+        <v>0.7736700038234695</v>
       </c>
       <c r="L9" s="3">
-        <v>0.06772599920288445</v>
+        <v>0.0685035405662703</v>
       </c>
       <c r="M9" s="3">
-        <v>-0.7477477315266444</v>
+        <v>-0.7473231739074477</v>
       </c>
       <c r="N9" s="3">
-        <v>1.446892231232934</v>
+        <v>1.447582411773152</v>
       </c>
       <c r="O9">
         <v>3</v>
@@ -2016,13 +2016,13 @@
         <v>38</v>
       </c>
       <c r="Z9" s="3">
-        <v>0.4507818961868427</v>
+        <v>0.451580293293589</v>
       </c>
       <c r="AA9">
         <v>-0.6999999999999998</v>
       </c>
       <c r="AB9" s="3">
-        <v>0.2757818961868428</v>
+        <v>0.276580293293589</v>
       </c>
       <c r="AC9">
         <v>6</v>
@@ -2057,16 +2057,16 @@
         <v>0.04822281934553629</v>
       </c>
       <c r="K10" s="3">
-        <v>-1.617525763680798</v>
+        <v>-1.617265779520059</v>
       </c>
       <c r="L10" s="3">
-        <v>-0.7691991583870909</v>
+        <v>-0.7691013138739796</v>
       </c>
       <c r="M10" s="3">
-        <v>3.105906328032698</v>
+        <v>3.105999795357508</v>
       </c>
       <c r="N10" s="3">
-        <v>2.337458416645688</v>
+        <v>2.337373947396912</v>
       </c>
       <c r="O10">
         <v>-2</v>
@@ -2102,13 +2102,13 @@
         <v>37</v>
       </c>
       <c r="Z10" s="3">
-        <v>0.6837916383460497</v>
+        <v>0.6838274393408871</v>
       </c>
       <c r="AA10">
         <v>-2</v>
       </c>
       <c r="AB10" s="3">
-        <v>0.1837916383460498</v>
+        <v>0.1838274393408871</v>
       </c>
       <c r="AC10">
         <v>7</v>
@@ -2143,16 +2143,16 @@
         <v>0.01576610693875313</v>
       </c>
       <c r="K11" s="3">
-        <v>-0.1359741487222176</v>
+        <v>-0.1357656929084249</v>
       </c>
       <c r="L11" s="3">
-        <v>1.715836418084274</v>
+        <v>1.715704772615058</v>
       </c>
       <c r="M11" s="3">
-        <v>0.3602341397317845</v>
+        <v>0.3602976634676422</v>
       </c>
       <c r="N11" s="3">
-        <v>-0.0372770061034126</v>
+        <v>-0.03724675310952241</v>
       </c>
       <c r="O11">
         <v>-1</v>
@@ -2188,13 +2188,13 @@
         <v>37</v>
       </c>
       <c r="Z11" s="3">
-        <v>0.3844744287757374</v>
+        <v>0.3844954086215743</v>
       </c>
       <c r="AA11">
         <v>-0.8999999999999998</v>
       </c>
       <c r="AB11" s="3">
-        <v>0.1594744287757374</v>
+        <v>0.1594954086215743</v>
       </c>
       <c r="AC11">
         <v>8</v>
@@ -2229,16 +2229,16 @@
         <v>0.01122599999999996</v>
       </c>
       <c r="K12" s="3">
-        <v>0.4988601241340718</v>
+        <v>0.4990465004196627</v>
       </c>
       <c r="L12" s="3">
-        <v>1.578430795196368</v>
+        <v>1.578311838967606</v>
       </c>
       <c r="M12" s="3">
-        <v>-0.2203522554562217</v>
+        <v>-0.220295063445048</v>
       </c>
       <c r="N12" s="3">
-        <v>-0.3694595338776333</v>
+        <v>-0.3694132333172667</v>
       </c>
       <c r="O12">
         <v>2</v>
@@ -2274,13 +2274,13 @@
         <v>38</v>
       </c>
       <c r="Z12" s="3">
-        <v>0.2583667896113326</v>
+        <v>0.2583958709210498</v>
       </c>
       <c r="AA12">
         <v>-0.5999999999999999</v>
       </c>
       <c r="AB12" s="3">
-        <v>0.1083667896113327</v>
+        <v>0.1083958709210499</v>
       </c>
       <c r="AC12">
         <v>9</v>
@@ -2315,16 +2315,16 @@
         <v>0.01238199999999989</v>
       </c>
       <c r="K13" s="3">
-        <v>1.231486582796208</v>
+        <v>1.231647478342577</v>
       </c>
       <c r="L13" s="3">
-        <v>0.7214436596089847</v>
+        <v>0.7214038450892849</v>
       </c>
       <c r="M13" s="3">
-        <v>-0.4457126145269887</v>
+        <v>-0.4456578802374567</v>
       </c>
       <c r="N13" s="3">
-        <v>-0.2848793670914223</v>
+        <v>-0.284837152555261</v>
       </c>
       <c r="O13">
         <v>3</v>
@@ -2360,13 +2360,13 @@
         <v>36</v>
       </c>
       <c r="Z13" s="3">
-        <v>0.1959468519470448</v>
+        <v>0.1959909194412265</v>
       </c>
       <c r="AA13">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB13" s="3">
-        <v>0.07094685194704484</v>
+        <v>0.0709909194412266</v>
       </c>
       <c r="AC13">
         <v>10</v>
@@ -2401,16 +2401,16 @@
         <v>0.006472000000000033</v>
       </c>
       <c r="K14" s="3">
-        <v>1.010639229851337</v>
+        <v>1.010807806465926</v>
       </c>
       <c r="L14" s="3">
-        <v>0.9659726744453141</v>
+        <v>0.9659102779715268</v>
       </c>
       <c r="M14" s="3">
-        <v>-0.5973831210870466</v>
+        <v>-0.597330040876732</v>
       </c>
       <c r="N14" s="3">
-        <v>-0.717291811474228</v>
+        <v>-0.717228707316048</v>
       </c>
       <c r="O14">
         <v>3</v>
@@ -2446,13 +2446,13 @@
         <v>36</v>
       </c>
       <c r="Z14" s="3">
-        <v>0.04288331758312258</v>
+        <v>0.04292931614709292</v>
       </c>
       <c r="AA14">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB14" s="3">
-        <v>-0.08211668241687736</v>
+        <v>-0.08207068385290703</v>
       </c>
       <c r="AC14">
         <v>11</v>
@@ -2487,16 +2487,16 @@
         <v>0.03876787002809845</v>
       </c>
       <c r="K15" s="3">
-        <v>-0.7838473796859533</v>
+        <v>-0.7836163908491562</v>
       </c>
       <c r="L15" s="3">
-        <v>-0.8589102675453107</v>
+        <v>-0.8588041383214895</v>
       </c>
       <c r="M15" s="3">
-        <v>1.470898853416422</v>
+        <v>1.470974489773659</v>
       </c>
       <c r="N15" s="3">
-        <v>1.64567538011964</v>
+        <v>1.645624330552329</v>
       </c>
       <c r="O15">
         <v>-2</v>
@@ -2532,13 +2532,13 @@
         <v>37</v>
       </c>
       <c r="Z15" s="3">
-        <v>0.3481235293611103</v>
+        <v>0.3481623636312134</v>
       </c>
       <c r="AA15">
         <v>-2</v>
       </c>
       <c r="AB15" s="3">
-        <v>-0.1518764706388896</v>
+        <v>-0.1518376363687866</v>
       </c>
       <c r="AC15">
         <v>12</v>
@@ -2573,16 +2573,16 @@
         <v>0.007047000000000025</v>
       </c>
       <c r="K16" s="3">
-        <v>0.9902658578084526</v>
+        <v>0.9904351430086702</v>
       </c>
       <c r="L16" s="3">
-        <v>0.4579882504354782</v>
+        <v>0.4579727656991295</v>
       </c>
       <c r="M16" s="3">
-        <v>-0.4025247642580569</v>
+        <v>-0.4024695589730282</v>
       </c>
       <c r="N16" s="3">
-        <v>-0.6752212267838531</v>
+        <v>-0.6751601550339068</v>
       </c>
       <c r="O16">
         <v>3</v>
@@ -2618,13 +2618,13 @@
         <v>36</v>
       </c>
       <c r="Z16" s="3">
-        <v>-0.0320068073199439</v>
+        <v>-0.03194865192146842</v>
       </c>
       <c r="AA16">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB16" s="3">
-        <v>-0.1570068073199438</v>
+        <v>-0.1569486519214684</v>
       </c>
       <c r="AC16">
         <v>13</v>
@@ -2659,16 +2659,16 @@
         <v>0.03255485138359315</v>
       </c>
       <c r="K17" s="3">
-        <v>-1.310295313274096</v>
+        <v>-1.310046014584643</v>
       </c>
       <c r="L17" s="3">
-        <v>-0.6457990673086956</v>
+        <v>-0.6457126186423838</v>
       </c>
       <c r="M17" s="3">
-        <v>1.273375261689994</v>
+        <v>1.273448743906157</v>
       </c>
       <c r="N17" s="3">
-        <v>1.191092202612611</v>
+        <v>1.191063113723993</v>
       </c>
       <c r="O17">
         <v>-2</v>
@@ -2704,13 +2704,13 @@
         <v>37</v>
       </c>
       <c r="Z17" s="3">
-        <v>0.2166482813007653</v>
+        <v>0.2166894766084366</v>
       </c>
       <c r="AA17">
         <v>-2</v>
       </c>
       <c r="AB17" s="3">
-        <v>-0.2833517186992346</v>
+        <v>-0.2833105233915634</v>
       </c>
       <c r="AC17">
         <v>14</v>
@@ -2745,16 +2745,16 @@
         <v>0.03622936028224144</v>
       </c>
       <c r="K18" s="3">
-        <v>-1.291551810994642</v>
+        <v>-1.291303164203968</v>
       </c>
       <c r="L18" s="3">
-        <v>-1.409668342757167</v>
+        <v>-1.409511351701771</v>
       </c>
       <c r="M18" s="3">
-        <v>1.485726060448545</v>
+        <v>1.485801858507458</v>
       </c>
       <c r="N18" s="3">
-        <v>1.459942181423256</v>
+        <v>1.459900104530916</v>
       </c>
       <c r="O18">
         <v>-2</v>
@@ -2790,13 +2790,13 @@
         <v>37</v>
       </c>
       <c r="Z18" s="3">
-        <v>0.1757187700557087</v>
+        <v>0.1757696069293094</v>
       </c>
       <c r="AA18">
         <v>-2</v>
       </c>
       <c r="AB18" s="3">
-        <v>-0.3242812299442913</v>
+        <v>-0.3242303930706905</v>
       </c>
       <c r="AC18">
         <v>15</v>
@@ -2831,16 +2831,16 @@
         <v>0.004156999999999966</v>
       </c>
       <c r="K19" s="3">
-        <v>1.026122992603929</v>
+        <v>1.02629103069344</v>
       </c>
       <c r="L19" s="3">
-        <v>0.1385107140239271</v>
+        <v>0.1385247326455501</v>
       </c>
       <c r="M19" s="3">
-        <v>-0.5032653221208153</v>
+        <v>-0.5032112154861893</v>
       </c>
       <c r="N19" s="3">
-        <v>-0.886671643749397</v>
+        <v>-0.8866003569389371</v>
       </c>
       <c r="O19">
         <v>3</v>
@@ -2876,13 +2876,13 @@
         <v>36</v>
       </c>
       <c r="Z19" s="3">
-        <v>-0.2029316253574076</v>
+        <v>-0.2028629038008068</v>
       </c>
       <c r="AA19">
         <v>-0.4999999999999998</v>
       </c>
       <c r="AB19" s="3">
-        <v>-0.3279316253574075</v>
+        <v>-0.3278629038008067</v>
       </c>
       <c r="AC19">
         <v>16</v>
@@ -2917,16 +2917,16 @@
         <v>0.008294000000000024</v>
       </c>
       <c r="K20" s="3">
-        <v>0.2152627852971158</v>
+        <v>0.2154590250946633</v>
       </c>
       <c r="L20" s="3">
-        <v>1.012153076628026</v>
+        <v>1.012086415450836</v>
       </c>
       <c r="M20" s="3">
-        <v>-0.7361812230312892</v>
+        <v>-0.7361296565170851</v>
       </c>
       <c r="N20" s="3">
-        <v>-0.5839829326814215</v>
+        <v>-0.5839262686063749</v>
       </c>
       <c r="O20">
         <v>2</v>
@@ -2962,13 +2962,13 @@
         <v>37</v>
       </c>
       <c r="Z20" s="3">
-        <v>-0.2304906461266385</v>
+        <v>-0.230446218798042</v>
       </c>
       <c r="AA20">
         <v>-0.5999999999999999</v>
       </c>
       <c r="AB20" s="3">
-        <v>-0.3804906461266385</v>
+        <v>-0.380446218798042</v>
       </c>
       <c r="AC20">
         <v>17</v>
@@ -3003,16 +3003,16 @@
         <v>0.02349157088044751</v>
       </c>
       <c r="K21" s="3">
-        <v>-1.127749899769848</v>
+        <v>-1.127506950007632</v>
       </c>
       <c r="L21" s="3">
-        <v>-0.6991714993395353</v>
+        <v>-0.6990801217946998</v>
       </c>
       <c r="M21" s="3">
-        <v>1.111208781579382</v>
+        <v>1.111280495249961</v>
       </c>
       <c r="N21" s="3">
-        <v>0.5279660982991882</v>
+        <v>0.5279690446904284</v>
       </c>
       <c r="O21">
         <v>-2</v>
@@ -3048,13 +3048,13 @@
         <v>37</v>
       </c>
       <c r="Z21" s="3">
-        <v>0.06300213126652165</v>
+        <v>0.0630498894343437</v>
       </c>
       <c r="AA21">
         <v>-2</v>
       </c>
       <c r="AB21" s="3">
-        <v>-0.4369978687334783</v>
+        <v>-0.4369501105656562</v>
       </c>
       <c r="AC21">
         <v>18</v>
@@ -3089,16 +3089,16 @@
         <v>0.005554000000000059</v>
       </c>
       <c r="K22" s="3">
-        <v>0.3921036546293556</v>
+        <v>0.3922937439036429</v>
       </c>
       <c r="L22" s="3">
-        <v>0.4042372905178948</v>
+        <v>0.404226769616655</v>
       </c>
       <c r="M22" s="3">
-        <v>-0.6054050543983434</v>
+        <v>-0.6053520616731535</v>
       </c>
       <c r="N22" s="3">
-        <v>-0.7844584145103387</v>
+        <v>-0.7843920655682309</v>
       </c>
       <c r="O22">
         <v>2</v>
@@ -3134,13 +3134,13 @@
         <v>38</v>
       </c>
       <c r="Z22" s="3">
-        <v>-0.2878988819948867</v>
+        <v>-0.2878371307850758</v>
       </c>
       <c r="AA22">
         <v>-0.5999999999999999</v>
       </c>
       <c r="AB22" s="3">
-        <v>-0.4378988819948866</v>
+        <v>-0.4378371307850757</v>
       </c>
       <c r="AC22">
         <v>19</v>
@@ -3175,16 +3175,16 @@
         <v>0.01051945602075555</v>
       </c>
       <c r="K23" s="3">
-        <v>-0.06833455353984018</v>
+        <v>-0.06812845023033598</v>
       </c>
       <c r="L23" s="3">
-        <v>0.4401974397585315</v>
+        <v>0.4401835979816907</v>
       </c>
       <c r="M23" s="3">
-        <v>-0.6662738219445684</v>
+        <v>-0.6662214930383745</v>
       </c>
       <c r="N23" s="3">
-        <v>-0.4211546961668106</v>
+        <v>-0.4211058982398339</v>
       </c>
       <c r="O23">
         <v>-1</v>
@@ -3220,13 +3220,13 @@
         <v>37</v>
       </c>
       <c r="Z23" s="3">
-        <v>-0.2327823386510476</v>
+        <v>-0.232736268279459</v>
       </c>
       <c r="AA23">
         <v>-0.8999999999999998</v>
       </c>
       <c r="AB23" s="3">
-        <v>-0.4577823386510476</v>
+        <v>-0.457736268279459</v>
       </c>
       <c r="AC23">
         <v>20</v>
@@ -3261,16 +3261,16 @@
         <v>0.01108500000000001</v>
       </c>
       <c r="K24" s="3">
-        <v>0.2682335526086162</v>
+        <v>0.2684279500835282</v>
       </c>
       <c r="L24" s="3">
-        <v>0.05674869048732174</v>
+        <v>0.05677025973136399</v>
       </c>
       <c r="M24" s="3">
-        <v>-0.5603516382430519</v>
+        <v>-0.5602981541769875</v>
       </c>
       <c r="N24" s="3">
-        <v>-0.3797759729060519</v>
+        <v>-0.3797291739638402</v>
       </c>
       <c r="O24">
         <v>2</v>
@@ -3306,13 +3306,13 @@
         <v>37</v>
       </c>
       <c r="Z24" s="3">
-        <v>-0.2818427872770104</v>
+        <v>-0.2817842688840067</v>
       </c>
       <c r="AA24">
         <v>-0.7999999999999998</v>
       </c>
       <c r="AB24" s="3">
-        <v>-0.4818427872770104</v>
+        <v>-0.4817842688840067</v>
       </c>
       <c r="AC24">
         <v>21</v>
@@ -3347,16 +3347,16 @@
         <v>0.0236741619528269</v>
       </c>
       <c r="K25" s="3">
-        <v>-0.8620811283306308</v>
+        <v>-0.861847418525018</v>
       </c>
       <c r="L25" s="3">
-        <v>-0.5958333862585479</v>
+        <v>-0.5957515518614923</v>
       </c>
       <c r="M25" s="3">
-        <v>0.4196250008701242</v>
+        <v>0.4196891723073138</v>
       </c>
       <c r="N25" s="3">
-        <v>0.5413255994717858</v>
+        <v>0.5413279004724192</v>
       </c>
       <c r="O25">
         <v>-2</v>
@@ -3392,13 +3392,13 @@
         <v>37</v>
       </c>
       <c r="Z25" s="3">
-        <v>6.44758533165507E-05</v>
+        <v>0.0001085406683122847</v>
       </c>
       <c r="AA25">
         <v>-2</v>
       </c>
       <c r="AB25" s="3">
-        <v>-0.4999355241466834</v>
+        <v>-0.4998914593316877</v>
       </c>
       <c r="AC25">
         <v>22</v>
@@ -3433,16 +3433,16 @@
         <v>0.002985254784476865</v>
       </c>
       <c r="K26" s="3">
-        <v>-0.722727263557299</v>
+        <v>-0.7224984004773891</v>
       </c>
       <c r="L26" s="3">
-        <v>0.8039627389190772</v>
+        <v>0.8039153038637875</v>
       </c>
       <c r="M26" s="3">
-        <v>-0.7494815195346708</v>
+        <v>-0.7494300980700517</v>
       </c>
       <c r="N26" s="3">
-        <v>-0.9724038286628003</v>
+        <v>-0.972328400174734</v>
       </c>
       <c r="O26">
         <v>-2</v>
@@ -3478,13 +3478,13 @@
         <v>37</v>
       </c>
       <c r="Z26" s="3">
-        <v>-0.2601803069995213</v>
+        <v>-0.26014240206166</v>
       </c>
       <c r="AA26">
         <v>-0.9999999999999998</v>
       </c>
       <c r="AB26" s="3">
-        <v>-0.5101803069995212</v>
+        <v>-0.5101424020616599</v>
       </c>
       <c r="AC26">
         <v>23</v>
@@ -3519,16 +3519,16 @@
         <v>0.007756000000000096</v>
       </c>
       <c r="K27" s="3">
-        <v>0.5518308914455723</v>
+        <v>0.5520154254085275</v>
       </c>
       <c r="L27" s="3">
-        <v>-0.07800723719337993</v>
+        <v>-0.07797322340497996</v>
       </c>
       <c r="M27" s="3">
-        <v>-0.8502605769814321</v>
+        <v>-0.8502102545870821</v>
       </c>
       <c r="N27" s="3">
-        <v>-0.6233463667047588</v>
+        <v>-0.6232878010025301</v>
       </c>
       <c r="O27">
         <v>2</v>
@@ -3564,13 +3564,13 @@
         <v>38</v>
       </c>
       <c r="Z27" s="3">
-        <v>-0.3869378541529166</v>
+        <v>-0.3868696886135535</v>
       </c>
       <c r="AA27">
         <v>-0.7999999999999998</v>
       </c>
       <c r="AB27" s="3">
-        <v>-0.5869378541529165</v>
+        <v>-0.5868696886135535</v>
       </c>
       <c r="AC27">
         <v>24</v>
@@ -3605,16 +3605,16 @@
         <v>0.005562999999999985</v>
       </c>
       <c r="K28" s="3">
-        <v>-0.006399502529470485</v>
+        <v>-0.006195553320278658</v>
       </c>
       <c r="L28" s="3">
-        <v>0.2463911617458371</v>
+        <v>0.2463952177406568</v>
       </c>
       <c r="M28" s="3">
-        <v>-0.6386121271753298</v>
+        <v>-0.6385594965978653</v>
       </c>
       <c r="N28" s="3">
-        <v>-0.783799918402147</v>
+        <v>-0.7837336012716464</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -3650,13 +3650,13 @@
         <v>37</v>
       </c>
       <c r="Z28" s="3">
-        <v>-0.4245127507780308</v>
+        <v>-0.4244536751828806</v>
       </c>
       <c r="AA28">
         <v>-0.7999999999999998</v>
       </c>
       <c r="AB28" s="3">
-        <v>-0.6245127507780308</v>
+        <v>-0.6244536751828806</v>
       </c>
       <c r="AC28">
         <v>25</v>
@@ -3691,16 +3691,16 @@
         <v>0.01152400000000009</v>
       </c>
       <c r="K29" s="3">
-        <v>-0.008029372292901271</v>
+        <v>-0.007825366396859119</v>
       </c>
       <c r="L29" s="3">
-        <v>-0.3952136062844697</v>
+        <v>-0.3951502988776096</v>
       </c>
       <c r="M29" s="3">
-        <v>-0.8964333326685434</v>
+        <v>-0.8963835138222948</v>
       </c>
       <c r="N29" s="3">
-        <v>-0.3476559960728726</v>
+        <v>-0.3476107488301645</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -3736,13 +3736,13 @@
         <v>37</v>
       </c>
       <c r="Z29" s="3">
-        <v>-0.4536893927457834</v>
+        <v>-0.4536279135873847</v>
       </c>
       <c r="AA29">
         <v>-1.2</v>
       </c>
       <c r="AB29" s="3">
-        <v>-0.7536893927457834</v>
+        <v>-0.7536279135873847</v>
       </c>
       <c r="AC29">
         <v>26</v>
@@ -3777,16 +3777,16 @@
         <v>0.004607999999999945</v>
       </c>
       <c r="K30" s="3">
-        <v>0.4222562452528251</v>
+        <v>0.4224452858203812</v>
       </c>
       <c r="L30" s="3">
-        <v>-0.2468306746810004</v>
+        <v>-0.246781070255568</v>
       </c>
       <c r="M30" s="3">
-        <v>-0.5601650816544118</v>
+        <v>-0.5601115955538095</v>
       </c>
       <c r="N30" s="3">
-        <v>-0.8536736721052953</v>
+        <v>-0.8536039794098153</v>
       </c>
       <c r="O30">
         <v>2</v>
@@ -3822,13 +3822,13 @@
         <v>37</v>
       </c>
       <c r="Z30" s="3">
-        <v>-0.5166595037493592</v>
+        <v>-0.5165867558991445</v>
       </c>
       <c r="AA30">
         <v>-1</v>
       </c>
       <c r="AB30" s="3">
-        <v>-0.7666595037493592</v>
+        <v>-0.7665867558991445</v>
       </c>
       <c r="AC30">
         <v>27</v>
@@ -3863,16 +3863,16 @@
         <v>0.01593287195180237</v>
       </c>
       <c r="K31" s="3">
-        <v>-1.012844081447978</v>
+        <v>-1.01260512810871</v>
       </c>
       <c r="L31" s="3">
-        <v>-1.364623524234685</v>
+        <v>-1.364470693012937</v>
       </c>
       <c r="M31" s="3">
-        <v>0.1736154893923004</v>
+        <v>0.1736769779135464</v>
       </c>
       <c r="N31" s="3">
-        <v>-0.02507543809492618</v>
+        <v>-0.02504577455248921</v>
       </c>
       <c r="O31">
         <v>-2</v>
@@ -3908,13 +3908,13 @@
         <v>37</v>
       </c>
       <c r="Z31" s="3">
-        <v>-0.2966299655373176</v>
+        <v>-0.2965682140893749</v>
       </c>
       <c r="AA31">
         <v>-2</v>
       </c>
       <c r="AB31" s="3">
-        <v>-0.7966299655373175</v>
+        <v>-0.7965682140893748</v>
       </c>
       <c r="AC31">
         <v>28</v>
@@ -3949,16 +3949,16 @@
         <v>0.003329317480264216</v>
       </c>
       <c r="K32" s="3">
-        <v>-0.2215423113023336</v>
+        <v>-0.2213308794288988</v>
       </c>
       <c r="L32" s="3">
-        <v>-0.3728804609666005</v>
+        <v>-0.3728192159982717</v>
       </c>
       <c r="M32" s="3">
-        <v>-1.09347122204017</v>
+        <v>-1.093423552038053</v>
       </c>
       <c r="N32" s="3">
-        <v>-0.9472300568681558</v>
+        <v>-0.9471558445120125</v>
       </c>
       <c r="O32">
         <v>-2</v>
@@ -3994,13 +3994,13 @@
         <v>37</v>
       </c>
       <c r="Z32" s="3">
-        <v>-0.4844280319534016</v>
+        <v>-0.4843724330688174</v>
       </c>
       <c r="AA32">
         <v>-1.4</v>
       </c>
       <c r="AB32" s="3">
-        <v>-0.8344280319534016</v>
+        <v>-0.8343724330688174</v>
       </c>
       <c r="AC32">
         <v>29</v>
@@ -4035,16 +4035,16 @@
         <v>0.01511745039651724</v>
       </c>
       <c r="K33" s="3">
-        <v>-0.6999090868692681</v>
+        <v>-0.6996810174052627</v>
       </c>
       <c r="L33" s="3">
-        <v>-1.29459586518713</v>
+        <v>-1.294449500933657</v>
       </c>
       <c r="M33" s="3">
-        <v>-0.2822241089360907</v>
+        <v>-0.2821675916833081</v>
       </c>
       <c r="N33" s="3">
-        <v>-0.08473676261663217</v>
+        <v>-0.08470421686639895</v>
       </c>
       <c r="O33">
         <v>-2</v>
@@ -4080,13 +4080,13 @@
         <v>37</v>
       </c>
       <c r="Z33" s="3">
-        <v>-0.3400401577067147</v>
+        <v>-0.3399806034064606</v>
       </c>
       <c r="AA33">
         <v>-2</v>
       </c>
       <c r="AB33" s="3">
-        <v>-0.8400401577067147</v>
+        <v>-0.8399806034064605</v>
       </c>
       <c r="AC33">
         <v>30</v>
@@ -4121,16 +4121,16 @@
         <v>0.01294211206956963</v>
       </c>
       <c r="K34" s="3">
-        <v>-0.7137629798584295</v>
+        <v>-0.7135344285561964</v>
       </c>
       <c r="L34" s="3">
-        <v>-1.137506792188559</v>
+        <v>-1.137374934917976</v>
       </c>
       <c r="M34" s="3">
-        <v>-0.2993245597098933</v>
+        <v>-0.2992682289501928</v>
       </c>
       <c r="N34" s="3">
-        <v>-0.2438980762063175</v>
+        <v>-0.2438578414551684</v>
       </c>
       <c r="O34">
         <v>-2</v>
@@ -4166,13 +4166,13 @@
         <v>37</v>
       </c>
       <c r="Z34" s="3">
-        <v>-0.349597873141724</v>
+        <v>-0.3495392040495664</v>
       </c>
       <c r="AA34">
         <v>-2</v>
       </c>
       <c r="AB34" s="3">
-        <v>-0.849597873141724</v>
+        <v>-0.8495392040495664</v>
       </c>
       <c r="AC34">
         <v>31</v>
@@ -4207,16 +4207,16 @@
         <v>0.01253918379911845</v>
       </c>
       <c r="K35" s="3">
-        <v>-0.6681266264823679</v>
+        <v>-0.6678996624119439</v>
       </c>
       <c r="L35" s="3">
-        <v>-0.8066734191747018</v>
+        <v>-0.8065721139596482</v>
       </c>
       <c r="M35" s="3">
-        <v>-0.7232166941190961</v>
+        <v>-0.7231649862171012</v>
       </c>
       <c r="N35" s="3">
-        <v>-0.2733788204257316</v>
+        <v>-0.2733371614750444</v>
       </c>
       <c r="O35">
         <v>-2</v>
@@ -4252,13 +4252,13 @@
         <v>37</v>
       </c>
       <c r="Z35" s="3">
-        <v>-0.3603466780777715</v>
+        <v>-0.360293754510281</v>
       </c>
       <c r="AA35">
         <v>-2</v>
       </c>
       <c r="AB35" s="3">
-        <v>-0.8603466780777715</v>
+        <v>-0.8602937545102809</v>
       </c>
       <c r="AC35">
         <v>32</v>
@@ -4272,37 +4272,37 @@
         <v>32</v>
       </c>
       <c r="D36" s="2">
-        <v>0.0083</v>
+        <v>0.0072</v>
       </c>
       <c r="E36" s="2">
-        <v>-0.3807</v>
+        <v>-0.3814</v>
       </c>
       <c r="F36" s="2">
-        <v>0.013811</v>
+        <v>0.013784</v>
       </c>
       <c r="G36" s="2">
-        <v>0.011368</v>
+        <v>0.011344</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36" s="2">
-        <v>0.01381100000000002</v>
+        <v>0.01378400000000002</v>
       </c>
       <c r="J36" s="2">
-        <v>0.01136800000000004</v>
+        <v>0.01134400000000002</v>
       </c>
       <c r="K36" s="3">
-        <v>0.009084260223121938</v>
+        <v>0.0003236989860431619</v>
       </c>
       <c r="L36" s="3">
-        <v>-2.081176813840214</v>
+        <v>-2.083607260313649</v>
       </c>
       <c r="M36" s="3">
-        <v>0.04203958645853996</v>
+        <v>0.03958109863427624</v>
       </c>
       <c r="N36" s="3">
-        <v>-0.3590699286149603</v>
+        <v>-0.3607800347619704</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -4338,13 +4338,13 @@
         <v>37</v>
       </c>
       <c r="Z36" s="3">
-        <v>-0.508099019996362</v>
+        <v>-0.5106878928251266</v>
       </c>
       <c r="AA36">
         <v>-1.8</v>
       </c>
       <c r="AB36" s="3">
-        <v>-0.9580990199963619</v>
+        <v>-0.9606878928251266</v>
       </c>
       <c r="AC36">
         <v>33</v>
@@ -4379,16 +4379,16 @@
         <v>0.009338999999999986</v>
       </c>
       <c r="K37" s="3">
-        <v>0.04657126478202991</v>
+        <v>0.04677337166858616</v>
       </c>
       <c r="L37" s="3">
-        <v>-0.7597359612185023</v>
+        <v>-0.7596389906200229</v>
       </c>
       <c r="M37" s="3">
-        <v>-0.8285267344054913</v>
+        <v>-0.8284761749874896</v>
       </c>
       <c r="N37" s="3">
-        <v>-0.5075242178963071</v>
+        <v>-0.5074712475023111</v>
       </c>
       <c r="O37">
         <v>1</v>
@@ -4424,13 +4424,13 @@
         <v>37</v>
       </c>
       <c r="Z37" s="3">
-        <v>-0.5569377291184711</v>
+        <v>-0.5568670855825151</v>
       </c>
       <c r="AA37">
         <v>-1.7</v>
       </c>
       <c r="AB37" s="3">
-        <v>-0.981937729118471</v>
+        <v>-0.981867085582515</v>
       </c>
       <c r="AC37">
         <v>34</v>
@@ -4465,16 +4465,16 @@
         <v>0.006153999999999993</v>
       </c>
       <c r="K38" s="3">
-        <v>0.005009585814544994</v>
+        <v>0.005213138215784543</v>
       </c>
       <c r="L38" s="3">
-        <v>-0.5507885677360661</v>
+        <v>-0.5507108931726582</v>
       </c>
       <c r="M38" s="3">
-        <v>-0.8067928918295504</v>
+        <v>-0.8067420953878971</v>
       </c>
       <c r="N38" s="3">
-        <v>-0.7405586739638648</v>
+        <v>-0.740494445795566</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -4510,13 +4510,13 @@
         <v>37</v>
       </c>
       <c r="Z38" s="3">
-        <v>-0.6025638256531579</v>
+        <v>-0.6024923827252203</v>
       </c>
       <c r="AA38">
         <v>-1.6</v>
       </c>
       <c r="AB38" s="3">
-        <v>-1.002563825653158</v>
+        <v>-1.00249238272522</v>
       </c>
       <c r="AC38">
         <v>35</v>
@@ -4551,16 +4551,16 @@
         <v>0.002719829125617412</v>
       </c>
       <c r="K39" s="3">
-        <v>-0.1058215580987482</v>
+        <v>-0.1056141509916865</v>
       </c>
       <c r="L39" s="3">
-        <v>-0.7847188017435761</v>
+        <v>-0.7846195240104687</v>
       </c>
       <c r="M39" s="3">
-        <v>-1.069856229596596</v>
+        <v>-1.069808302055494</v>
       </c>
       <c r="N39" s="3">
-        <v>-0.991824024593314</v>
+        <v>-0.991747657925605</v>
       </c>
       <c r="O39">
         <v>-1</v>
@@ -4596,13 +4596,13 @@
         <v>37</v>
       </c>
       <c r="Z39" s="3">
-        <v>-0.6914271849527744</v>
+        <v>-0.6913583105630441</v>
       </c>
       <c r="AA39">
         <v>-1.9</v>
       </c>
       <c r="AB39" s="3">
-        <v>-1.166427184952775</v>
+        <v>-1.166358310563044</v>
       </c>
       <c r="AC39">
         <v>36</v>
@@ -4728,10 +4728,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.8974637158227678</v>
+        <v>0.8974503214619483</v>
       </c>
       <c r="D2">
-        <v>1.022463715822768</v>
+        <v>1.022450321461948</v>
       </c>
       <c r="E2">
         <v>-0.4999999999999998</v>
@@ -4766,10 +4766,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.7515903722702155</v>
+        <v>0.7515949802543345</v>
       </c>
       <c r="D3">
-        <v>1.001590372270216</v>
+        <v>1.001594980254334</v>
       </c>
       <c r="E3">
         <v>-0.9999999999999998</v>
@@ -4804,10 +4804,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.66316073431648</v>
+        <v>0.6631894861321259</v>
       </c>
       <c r="D4">
-        <v>0.7881607343164799</v>
+        <v>0.7881894861321258</v>
       </c>
       <c r="E4">
         <v>-0.4999999999999998</v>
@@ -4842,10 +4842,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.550428181377655</v>
+        <v>0.5504359545535373</v>
       </c>
       <c r="D5">
-        <v>0.800428181377655</v>
+        <v>0.8004359545535373</v>
       </c>
       <c r="E5">
         <v>-0.9999999999999998</v>
@@ -4880,10 +4880,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.5204715599289735</v>
+        <v>0.5205144937098669</v>
       </c>
       <c r="D6">
-        <v>0.6454715599289735</v>
+        <v>0.6455144937098668</v>
       </c>
       <c r="E6">
         <v>-0.4999999999999998</v>
@@ -4918,25 +4918,25 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.2757818961868428</v>
+        <v>0.276580293293589</v>
       </c>
       <c r="D7">
-        <v>0.4507818961868427</v>
+        <v>0.451580293293589</v>
       </c>
       <c r="E7">
         <v>-0.6999999999999998</v>
       </c>
       <c r="F7">
-        <v>0.1019</v>
+        <v>0.1021</v>
       </c>
       <c r="G7">
-        <v>0.187</v>
+        <v>0.1872</v>
       </c>
       <c r="H7">
-        <v>0.005344</v>
+        <v>0.005347999999999999</v>
       </c>
       <c r="I7">
-        <v>0.036051</v>
+        <v>0.036061</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -4956,10 +4956,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.1837916383460498</v>
+        <v>0.1838274393408871</v>
       </c>
       <c r="D8">
-        <v>0.6837916383460497</v>
+        <v>0.6838274393408871</v>
       </c>
       <c r="E8">
         <v>-2</v>
@@ -4994,10 +4994,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.1594744287757374</v>
+        <v>0.1594954086215743</v>
       </c>
       <c r="D9">
-        <v>0.3844744287757374</v>
+        <v>0.3844954086215743</v>
       </c>
       <c r="E9">
         <v>-0.8999999999999998</v>
@@ -5032,10 +5032,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.1083667896113327</v>
+        <v>0.1083958709210499</v>
       </c>
       <c r="D10">
-        <v>0.2583667896113326</v>
+        <v>0.2583958709210498</v>
       </c>
       <c r="E10">
         <v>-0.5999999999999999</v>
@@ -5070,10 +5070,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.07094685194704484</v>
+        <v>0.0709909194412266</v>
       </c>
       <c r="D11">
-        <v>0.1959468519470448</v>
+        <v>0.1959909194412265</v>
       </c>
       <c r="E11">
         <v>-0.4999999999999998</v>
@@ -5108,10 +5108,10 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>-0.08211668241687736</v>
+        <v>-0.08207068385290703</v>
       </c>
       <c r="D12">
-        <v>0.04288331758312258</v>
+        <v>0.04292931614709292</v>
       </c>
       <c r="E12">
         <v>-0.4999999999999998</v>
@@ -5146,10 +5146,10 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>-0.1518764706388896</v>
+        <v>-0.1518376363687866</v>
       </c>
       <c r="D13">
-        <v>0.3481235293611103</v>
+        <v>0.3481623636312134</v>
       </c>
       <c r="E13">
         <v>-2</v>
@@ -5184,10 +5184,10 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-0.1570068073199438</v>
+        <v>-0.1569486519214684</v>
       </c>
       <c r="D14">
-        <v>-0.0320068073199439</v>
+        <v>-0.03194865192146842</v>
       </c>
       <c r="E14">
         <v>-0.4999999999999998</v>
@@ -5222,10 +5222,10 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>-0.2833517186992346</v>
+        <v>-0.2833105233915634</v>
       </c>
       <c r="D15">
-        <v>0.2166482813007653</v>
+        <v>0.2166894766084366</v>
       </c>
       <c r="E15">
         <v>-2</v>
@@ -5260,10 +5260,10 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>-0.3242812299442913</v>
+        <v>-0.3242303930706905</v>
       </c>
       <c r="D16">
-        <v>0.1757187700557087</v>
+        <v>0.1757696069293094</v>
       </c>
       <c r="E16">
         <v>-2</v>
@@ -5298,10 +5298,10 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>-0.3279316253574075</v>
+        <v>-0.3278629038008067</v>
       </c>
       <c r="D17">
-        <v>-0.2029316253574076</v>
+        <v>-0.2028629038008068</v>
       </c>
       <c r="E17">
         <v>-0.4999999999999998</v>
@@ -5336,10 +5336,10 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>-0.3804906461266385</v>
+        <v>-0.380446218798042</v>
       </c>
       <c r="D18">
-        <v>-0.2304906461266385</v>
+        <v>-0.230446218798042</v>
       </c>
       <c r="E18">
         <v>-0.5999999999999999</v>
@@ -5374,10 +5374,10 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>-0.4369978687334783</v>
+        <v>-0.4369501105656562</v>
       </c>
       <c r="D19">
-        <v>0.06300213126652165</v>
+        <v>0.0630498894343437</v>
       </c>
       <c r="E19">
         <v>-2</v>
@@ -5412,10 +5412,10 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>-0.4378988819948866</v>
+        <v>-0.4378371307850757</v>
       </c>
       <c r="D20">
-        <v>-0.2878988819948867</v>
+        <v>-0.2878371307850758</v>
       </c>
       <c r="E20">
         <v>-0.5999999999999999</v>
@@ -5450,10 +5450,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>-0.4577823386510476</v>
+        <v>-0.457736268279459</v>
       </c>
       <c r="D21">
-        <v>-0.2327823386510476</v>
+        <v>-0.232736268279459</v>
       </c>
       <c r="E21">
         <v>-0.8999999999999998</v>
@@ -5488,10 +5488,10 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>-0.4818427872770104</v>
+        <v>-0.4817842688840067</v>
       </c>
       <c r="D22">
-        <v>-0.2818427872770104</v>
+        <v>-0.2817842688840067</v>
       </c>
       <c r="E22">
         <v>-0.7999999999999998</v>
@@ -5526,10 +5526,10 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>-0.4999355241466834</v>
+        <v>-0.4998914593316877</v>
       </c>
       <c r="D23">
-        <v>6.44758533165507E-05</v>
+        <v>0.0001085406683122847</v>
       </c>
       <c r="E23">
         <v>-2</v>
@@ -5564,10 +5564,10 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>-0.5101803069995212</v>
+        <v>-0.5101424020616599</v>
       </c>
       <c r="D24">
-        <v>-0.2601803069995213</v>
+        <v>-0.26014240206166</v>
       </c>
       <c r="E24">
         <v>-0.9999999999999998</v>
@@ -5602,10 +5602,10 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>-0.5869378541529165</v>
+        <v>-0.5868696886135535</v>
       </c>
       <c r="D25">
-        <v>-0.3869378541529166</v>
+        <v>-0.3868696886135535</v>
       </c>
       <c r="E25">
         <v>-0.7999999999999998</v>
@@ -5640,10 +5640,10 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>-0.6245127507780308</v>
+        <v>-0.6244536751828806</v>
       </c>
       <c r="D26">
-        <v>-0.4245127507780308</v>
+        <v>-0.4244536751828806</v>
       </c>
       <c r="E26">
         <v>-0.7999999999999998</v>
@@ -5730,10 +5730,10 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>-1.166427184952775</v>
+        <v>-1.166358310563044</v>
       </c>
       <c r="D2">
-        <v>-0.6914271849527744</v>
+        <v>-0.6913583105630441</v>
       </c>
       <c r="E2">
         <v>-1.9</v>
@@ -5768,10 +5768,10 @@
         <v>34</v>
       </c>
       <c r="C3">
-        <v>-1.002563825653158</v>
+        <v>-1.00249238272522</v>
       </c>
       <c r="D3">
-        <v>-0.6025638256531579</v>
+        <v>-0.6024923827252203</v>
       </c>
       <c r="E3">
         <v>-1.6</v>
@@ -5806,10 +5806,10 @@
         <v>33</v>
       </c>
       <c r="C4">
-        <v>-0.981937729118471</v>
+        <v>-0.981867085582515</v>
       </c>
       <c r="D4">
-        <v>-0.5569377291184711</v>
+        <v>-0.5568670855825151</v>
       </c>
       <c r="E4">
         <v>-1.7</v>
@@ -5844,25 +5844,25 @@
         <v>32</v>
       </c>
       <c r="C5">
-        <v>-0.9580990199963619</v>
+        <v>-0.9606878928251266</v>
       </c>
       <c r="D5">
-        <v>-0.508099019996362</v>
+        <v>-0.5106878928251266</v>
       </c>
       <c r="E5">
         <v>-1.8</v>
       </c>
       <c r="F5">
-        <v>0.0083</v>
+        <v>0.0072</v>
       </c>
       <c r="G5">
-        <v>-0.3807</v>
+        <v>-0.3814</v>
       </c>
       <c r="H5">
-        <v>0.013811</v>
+        <v>0.013784</v>
       </c>
       <c r="I5">
-        <v>0.011368</v>
+        <v>0.011344</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -5882,10 +5882,10 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>-0.8603466780777715</v>
+        <v>-0.8602937545102809</v>
       </c>
       <c r="D6">
-        <v>-0.3603466780777715</v>
+        <v>-0.360293754510281</v>
       </c>
       <c r="E6">
         <v>-2</v>
@@ -5920,10 +5920,10 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <v>-0.849597873141724</v>
+        <v>-0.8495392040495664</v>
       </c>
       <c r="D7">
-        <v>-0.349597873141724</v>
+        <v>-0.3495392040495664</v>
       </c>
       <c r="E7">
         <v>-2</v>
@@ -5958,10 +5958,10 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>-0.8400401577067147</v>
+        <v>-0.8399806034064605</v>
       </c>
       <c r="D8">
-        <v>-0.3400401577067147</v>
+        <v>-0.3399806034064606</v>
       </c>
       <c r="E8">
         <v>-2</v>
@@ -5996,10 +5996,10 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>-0.8344280319534016</v>
+        <v>-0.8343724330688174</v>
       </c>
       <c r="D9">
-        <v>-0.4844280319534016</v>
+        <v>-0.4843724330688174</v>
       </c>
       <c r="E9">
         <v>-1.4</v>
@@ -6034,10 +6034,10 @@
         <v>27</v>
       </c>
       <c r="C10">
-        <v>-0.7966299655373175</v>
+        <v>-0.7965682140893748</v>
       </c>
       <c r="D10">
-        <v>-0.2966299655373176</v>
+        <v>-0.2965682140893749</v>
       </c>
       <c r="E10">
         <v>-2</v>
@@ -6072,10 +6072,10 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <v>-0.7666595037493592</v>
+        <v>-0.7665867558991445</v>
       </c>
       <c r="D11">
-        <v>-0.5166595037493592</v>
+        <v>-0.5165867558991445</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -6110,10 +6110,10 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>-0.7536893927457834</v>
+        <v>-0.7536279135873847</v>
       </c>
       <c r="D12">
-        <v>-0.4536893927457834</v>
+        <v>-0.4536279135873847</v>
       </c>
       <c r="E12">
         <v>-1.2</v>
@@ -6148,10 +6148,10 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>-0.6245127507780308</v>
+        <v>-0.6244536751828806</v>
       </c>
       <c r="D13">
-        <v>-0.4245127507780308</v>
+        <v>-0.4244536751828806</v>
       </c>
       <c r="E13">
         <v>-0.7999999999999998</v>
@@ -6186,10 +6186,10 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>-0.5869378541529165</v>
+        <v>-0.5868696886135535</v>
       </c>
       <c r="D14">
-        <v>-0.3869378541529166</v>
+        <v>-0.3868696886135535</v>
       </c>
       <c r="E14">
         <v>-0.7999999999999998</v>
@@ -6224,10 +6224,10 @@
         <v>22</v>
       </c>
       <c r="C15">
-        <v>-0.5101803069995212</v>
+        <v>-0.5101424020616599</v>
       </c>
       <c r="D15">
-        <v>-0.2601803069995213</v>
+        <v>-0.26014240206166</v>
       </c>
       <c r="E15">
         <v>-0.9999999999999998</v>
@@ -6262,10 +6262,10 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>-0.4999355241466834</v>
+        <v>-0.4998914593316877</v>
       </c>
       <c r="D16">
-        <v>6.44758533165507E-05</v>
+        <v>0.0001085406683122847</v>
       </c>
       <c r="E16">
         <v>-2</v>
@@ -6300,10 +6300,10 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>-0.4818427872770104</v>
+        <v>-0.4817842688840067</v>
       </c>
       <c r="D17">
-        <v>-0.2818427872770104</v>
+        <v>-0.2817842688840067</v>
       </c>
       <c r="E17">
         <v>-0.7999999999999998</v>
@@ -6338,10 +6338,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>-0.4577823386510476</v>
+        <v>-0.457736268279459</v>
       </c>
       <c r="D18">
-        <v>-0.2327823386510476</v>
+        <v>-0.232736268279459</v>
       </c>
       <c r="E18">
         <v>-0.8999999999999998</v>
@@ -6376,10 +6376,10 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>-0.4378988819948866</v>
+        <v>-0.4378371307850757</v>
       </c>
       <c r="D19">
-        <v>-0.2878988819948867</v>
+        <v>-0.2878371307850758</v>
       </c>
       <c r="E19">
         <v>-0.5999999999999999</v>
@@ -6414,10 +6414,10 @@
         <v>17</v>
       </c>
       <c r="C20">
-        <v>-0.4369978687334783</v>
+        <v>-0.4369501105656562</v>
       </c>
       <c r="D20">
-        <v>0.06300213126652165</v>
+        <v>0.0630498894343437</v>
       </c>
       <c r="E20">
         <v>-2</v>
@@ -6452,10 +6452,10 @@
         <v>16</v>
       </c>
       <c r="C21">
-        <v>-0.3804906461266385</v>
+        <v>-0.380446218798042</v>
       </c>
       <c r="D21">
-        <v>-0.2304906461266385</v>
+        <v>-0.230446218798042</v>
       </c>
       <c r="E21">
         <v>-0.5999999999999999</v>
@@ -6490,10 +6490,10 @@
         <v>15</v>
       </c>
       <c r="C22">
-        <v>-0.3279316253574075</v>
+        <v>-0.3278629038008067</v>
       </c>
       <c r="D22">
-        <v>-0.2029316253574076</v>
+        <v>-0.2028629038008068</v>
       </c>
       <c r="E22">
         <v>-0.4999999999999998</v>
@@ -6528,10 +6528,10 @@
         <v>14</v>
       </c>
       <c r="C23">
-        <v>-0.3242812299442913</v>
+        <v>-0.3242303930706905</v>
       </c>
       <c r="D23">
-        <v>0.1757187700557087</v>
+        <v>0.1757696069293094</v>
       </c>
       <c r="E23">
         <v>-2</v>
@@ -6566,10 +6566,10 @@
         <v>13</v>
       </c>
       <c r="C24">
-        <v>-0.2833517186992346</v>
+        <v>-0.2833105233915634</v>
       </c>
       <c r="D24">
-        <v>0.2166482813007653</v>
+        <v>0.2166894766084366</v>
       </c>
       <c r="E24">
         <v>-2</v>
@@ -6604,10 +6604,10 @@
         <v>12</v>
       </c>
       <c r="C25">
-        <v>-0.1570068073199438</v>
+        <v>-0.1569486519214684</v>
       </c>
       <c r="D25">
-        <v>-0.0320068073199439</v>
+        <v>-0.03194865192146842</v>
       </c>
       <c r="E25">
         <v>-0.4999999999999998</v>
@@ -6642,10 +6642,10 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <v>-0.1518764706388896</v>
+        <v>-0.1518376363687866</v>
       </c>
       <c r="D26">
-        <v>0.3481235293611103</v>
+        <v>0.3481623636312134</v>
       </c>
       <c r="E26">
         <v>-2</v>
@@ -6795,16 +6795,16 @@
         <v>0.01152200000000003</v>
       </c>
       <c r="I2">
-        <v>1.251859954839093</v>
+        <v>1.252020141799833</v>
       </c>
       <c r="J2">
-        <v>3.23751852279332</v>
+        <v>3.237246351851301</v>
       </c>
       <c r="K2">
-        <v>0.3444478166354552</v>
+        <v>0.3445111682097665</v>
       </c>
       <c r="L2">
-        <v>-0.347802328541365</v>
+        <v>-0.3477570742294109</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -6840,13 +6840,13 @@
         <v>36</v>
       </c>
       <c r="X2">
-        <v>1.022463715822768</v>
+        <v>1.022450321461948</v>
       </c>
       <c r="Y2">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z2">
-        <v>0.8974637158227678</v>
+        <v>0.8974503214619483</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -6878,16 +6878,16 @@
         <v>0.04519641354342707</v>
       </c>
       <c r="I3">
-        <v>-1.482246573316043</v>
+        <v>-1.481991294163881</v>
       </c>
       <c r="J3">
-        <v>1.296806047459171</v>
+        <v>1.296713098929854</v>
       </c>
       <c r="K3">
-        <v>2.544420525329981</v>
+        <v>2.544507869236216</v>
       </c>
       <c r="L3">
-        <v>2.116027700810766</v>
+        <v>2.115953928765592</v>
       </c>
       <c r="M3">
         <v>-2</v>
@@ -6923,13 +6923,13 @@
         <v>37</v>
       </c>
       <c r="X3">
-        <v>1.001590372270216</v>
+        <v>1.001594980254334</v>
       </c>
       <c r="Y3">
         <v>-0.9999999999999998</v>
       </c>
       <c r="Z3">
-        <v>0.7515903722702155</v>
+        <v>0.7515949802543345</v>
       </c>
       <c r="AA3">
         <v>2</v>
@@ -6961,16 +6961,16 @@
         <v>0.007770999999999972</v>
       </c>
       <c r="I4">
-        <v>4.166882026735045</v>
+        <v>4.166940829263979</v>
       </c>
       <c r="J4">
-        <v>0.9288769415444466</v>
+        <v>0.9288179708160164</v>
       </c>
       <c r="K4">
-        <v>0.1817704713459624</v>
+        <v>0.181832048803327</v>
       </c>
       <c r="L4">
-        <v>-0.622248873191106</v>
+        <v>-0.6221903605082224</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -7006,13 +7006,13 @@
         <v>36</v>
       </c>
       <c r="X4">
-        <v>0.7881607343164799</v>
+        <v>0.7881894861321258</v>
       </c>
       <c r="Y4">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z4">
-        <v>0.66316073431648</v>
+        <v>0.6631894861321259</v>
       </c>
       <c r="AA4">
         <v>3</v>
@@ -7044,16 +7044,16 @@
         <v>0.05321653603768906</v>
       </c>
       <c r="I5">
-        <v>-0.7088733705681374</v>
+        <v>-0.7086449893264553</v>
       </c>
       <c r="J5">
-        <v>0.4428471349657365</v>
+        <v>0.4428330484927987</v>
       </c>
       <c r="K5">
-        <v>1.07952337253551</v>
+        <v>1.079594740653234</v>
       </c>
       <c r="L5">
-        <v>2.702829861892565</v>
+        <v>2.702727741737839</v>
       </c>
       <c r="M5">
         <v>-2</v>
@@ -7089,13 +7089,13 @@
         <v>37</v>
       </c>
       <c r="X5">
-        <v>0.800428181377655</v>
+        <v>0.8004359545535373</v>
       </c>
       <c r="Y5">
         <v>-0.9999999999999998</v>
       </c>
       <c r="Z5">
-        <v>0.550428181377655</v>
+        <v>0.5504359545535373</v>
       </c>
       <c r="AA5">
         <v>4</v>
@@ -7127,16 +7127,16 @@
         <v>0.0164979999999999</v>
       </c>
       <c r="I6">
-        <v>1.555830665718934</v>
+        <v>1.555980280582088</v>
       </c>
       <c r="J6">
-        <v>0.6332466619977388</v>
+        <v>0.633214992362408</v>
       </c>
       <c r="K6">
-        <v>0.8790257213683046</v>
+        <v>0.8790949029106326</v>
       </c>
       <c r="L6">
-        <v>0.01627285305742284</v>
+        <v>0.01630051908525421</v>
       </c>
       <c r="M6">
         <v>3</v>
@@ -7172,13 +7172,13 @@
         <v>36</v>
       </c>
       <c r="X6">
-        <v>0.6454715599289735</v>
+        <v>0.6455144937098668</v>
       </c>
       <c r="Y6">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z6">
-        <v>0.5204715599289735</v>
+        <v>0.5205144937098669</v>
       </c>
       <c r="AA6">
         <v>5</v>
@@ -7189,37 +7189,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1019</v>
+        <v>0.1021</v>
       </c>
       <c r="C7">
-        <v>0.187</v>
+        <v>0.1872</v>
       </c>
       <c r="D7">
-        <v>0.005344</v>
+        <v>0.005347999999999999</v>
       </c>
       <c r="E7">
-        <v>0.036051</v>
+        <v>0.036061</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.005344000000000015</v>
+        <v>0.005347999999999908</v>
       </c>
       <c r="H7">
-        <v>0.03605100000000006</v>
+        <v>0.0360609999999999</v>
       </c>
       <c r="I7">
-        <v>0.7718633095087277</v>
+        <v>0.7736700038234695</v>
       </c>
       <c r="J7">
-        <v>0.06772599920288445</v>
+        <v>0.0685035405662703</v>
       </c>
       <c r="K7">
-        <v>-0.7477477315266444</v>
+        <v>-0.7473231739074477</v>
       </c>
       <c r="L7">
-        <v>1.446892231232934</v>
+        <v>1.447582411773152</v>
       </c>
       <c r="M7">
         <v>3</v>
@@ -7255,13 +7255,13 @@
         <v>38</v>
       </c>
       <c r="X7">
-        <v>0.4507818961868427</v>
+        <v>0.451580293293589</v>
       </c>
       <c r="Y7">
         <v>-0.6999999999999998</v>
       </c>
       <c r="Z7">
-        <v>0.2757818961868428</v>
+        <v>0.276580293293589</v>
       </c>
       <c r="AA7">
         <v>6</v>
@@ -7293,16 +7293,16 @@
         <v>0.04822281934553629</v>
       </c>
       <c r="I8">
-        <v>-1.617525763680798</v>
+        <v>-1.617265779520059</v>
       </c>
       <c r="J8">
-        <v>-0.7691991583870909</v>
+        <v>-0.7691013138739796</v>
       </c>
       <c r="K8">
-        <v>3.105906328032698</v>
+        <v>3.105999795357508</v>
       </c>
       <c r="L8">
-        <v>2.337458416645688</v>
+        <v>2.337373947396912</v>
       </c>
       <c r="M8">
         <v>-2</v>
@@ -7338,13 +7338,13 @@
         <v>37</v>
       </c>
       <c r="X8">
-        <v>0.6837916383460497</v>
+        <v>0.6838274393408871</v>
       </c>
       <c r="Y8">
         <v>-2</v>
       </c>
       <c r="Z8">
-        <v>0.1837916383460498</v>
+        <v>0.1838274393408871</v>
       </c>
       <c r="AA8">
         <v>7</v>
@@ -7376,16 +7376,16 @@
         <v>0.01576610693875313</v>
       </c>
       <c r="I9">
-        <v>-0.1359741487222176</v>
+        <v>-0.1357656929084249</v>
       </c>
       <c r="J9">
-        <v>1.715836418084274</v>
+        <v>1.715704772615058</v>
       </c>
       <c r="K9">
-        <v>0.3602341397317845</v>
+        <v>0.3602976634676422</v>
       </c>
       <c r="L9">
-        <v>-0.0372770061034126</v>
+        <v>-0.03724675310952241</v>
       </c>
       <c r="M9">
         <v>-1</v>
@@ -7421,13 +7421,13 @@
         <v>37</v>
       </c>
       <c r="X9">
-        <v>0.3844744287757374</v>
+        <v>0.3844954086215743</v>
       </c>
       <c r="Y9">
         <v>-0.8999999999999998</v>
       </c>
       <c r="Z9">
-        <v>0.1594744287757374</v>
+        <v>0.1594954086215743</v>
       </c>
       <c r="AA9">
         <v>8</v>
@@ -7459,16 +7459,16 @@
         <v>0.01122599999999996</v>
       </c>
       <c r="I10">
-        <v>0.4988601241340718</v>
+        <v>0.4990465004196627</v>
       </c>
       <c r="J10">
-        <v>1.578430795196368</v>
+        <v>1.578311838967606</v>
       </c>
       <c r="K10">
-        <v>-0.2203522554562217</v>
+        <v>-0.220295063445048</v>
       </c>
       <c r="L10">
-        <v>-0.3694595338776333</v>
+        <v>-0.3694132333172667</v>
       </c>
       <c r="M10">
         <v>2</v>
@@ -7504,13 +7504,13 @@
         <v>38</v>
       </c>
       <c r="X10">
-        <v>0.2583667896113326</v>
+        <v>0.2583958709210498</v>
       </c>
       <c r="Y10">
         <v>-0.5999999999999999</v>
       </c>
       <c r="Z10">
-        <v>0.1083667896113327</v>
+        <v>0.1083958709210499</v>
       </c>
       <c r="AA10">
         <v>9</v>
@@ -7542,16 +7542,16 @@
         <v>0.01238199999999989</v>
       </c>
       <c r="I11">
-        <v>1.231486582796208</v>
+        <v>1.231647478342577</v>
       </c>
       <c r="J11">
-        <v>0.7214436596089847</v>
+        <v>0.7214038450892849</v>
       </c>
       <c r="K11">
-        <v>-0.4457126145269887</v>
+        <v>-0.4456578802374567</v>
       </c>
       <c r="L11">
-        <v>-0.2848793670914223</v>
+        <v>-0.284837152555261</v>
       </c>
       <c r="M11">
         <v>3</v>
@@ -7587,13 +7587,13 @@
         <v>36</v>
       </c>
       <c r="X11">
-        <v>0.1959468519470448</v>
+        <v>0.1959909194412265</v>
       </c>
       <c r="Y11">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z11">
-        <v>0.07094685194704484</v>
+        <v>0.0709909194412266</v>
       </c>
       <c r="AA11">
         <v>10</v>
@@ -7625,16 +7625,16 @@
         <v>0.006472000000000033</v>
       </c>
       <c r="I12">
-        <v>1.010639229851337</v>
+        <v>1.010807806465926</v>
       </c>
       <c r="J12">
-        <v>0.9659726744453141</v>
+        <v>0.9659102779715268</v>
       </c>
       <c r="K12">
-        <v>-0.5973831210870466</v>
+        <v>-0.597330040876732</v>
       </c>
       <c r="L12">
-        <v>-0.717291811474228</v>
+        <v>-0.717228707316048</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -7670,13 +7670,13 @@
         <v>36</v>
       </c>
       <c r="X12">
-        <v>0.04288331758312258</v>
+        <v>0.04292931614709292</v>
       </c>
       <c r="Y12">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z12">
-        <v>-0.08211668241687736</v>
+        <v>-0.08207068385290703</v>
       </c>
       <c r="AA12">
         <v>11</v>
@@ -7708,16 +7708,16 @@
         <v>0.03876787002809845</v>
       </c>
       <c r="I13">
-        <v>-0.7838473796859533</v>
+        <v>-0.7836163908491562</v>
       </c>
       <c r="J13">
-        <v>-0.8589102675453107</v>
+        <v>-0.8588041383214895</v>
       </c>
       <c r="K13">
-        <v>1.470898853416422</v>
+        <v>1.470974489773659</v>
       </c>
       <c r="L13">
-        <v>1.64567538011964</v>
+        <v>1.645624330552329</v>
       </c>
       <c r="M13">
         <v>-2</v>
@@ -7753,13 +7753,13 @@
         <v>37</v>
       </c>
       <c r="X13">
-        <v>0.3481235293611103</v>
+        <v>0.3481623636312134</v>
       </c>
       <c r="Y13">
         <v>-2</v>
       </c>
       <c r="Z13">
-        <v>-0.1518764706388896</v>
+        <v>-0.1518376363687866</v>
       </c>
       <c r="AA13">
         <v>12</v>
@@ -7791,16 +7791,16 @@
         <v>0.007047000000000025</v>
       </c>
       <c r="I14">
-        <v>0.9902658578084526</v>
+        <v>0.9904351430086702</v>
       </c>
       <c r="J14">
-        <v>0.4579882504354782</v>
+        <v>0.4579727656991295</v>
       </c>
       <c r="K14">
-        <v>-0.4025247642580569</v>
+        <v>-0.4024695589730282</v>
       </c>
       <c r="L14">
-        <v>-0.6752212267838531</v>
+        <v>-0.6751601550339068</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -7836,13 +7836,13 @@
         <v>36</v>
       </c>
       <c r="X14">
-        <v>-0.0320068073199439</v>
+        <v>-0.03194865192146842</v>
       </c>
       <c r="Y14">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z14">
-        <v>-0.1570068073199438</v>
+        <v>-0.1569486519214684</v>
       </c>
       <c r="AA14">
         <v>13</v>
@@ -7874,16 +7874,16 @@
         <v>0.03255485138359315</v>
       </c>
       <c r="I15">
-        <v>-1.310295313274096</v>
+        <v>-1.310046014584643</v>
       </c>
       <c r="J15">
-        <v>-0.6457990673086956</v>
+        <v>-0.6457126186423838</v>
       </c>
       <c r="K15">
-        <v>1.273375261689994</v>
+        <v>1.273448743906157</v>
       </c>
       <c r="L15">
-        <v>1.191092202612611</v>
+        <v>1.191063113723993</v>
       </c>
       <c r="M15">
         <v>-2</v>
@@ -7919,13 +7919,13 @@
         <v>37</v>
       </c>
       <c r="X15">
-        <v>0.2166482813007653</v>
+        <v>0.2166894766084366</v>
       </c>
       <c r="Y15">
         <v>-2</v>
       </c>
       <c r="Z15">
-        <v>-0.2833517186992346</v>
+        <v>-0.2833105233915634</v>
       </c>
       <c r="AA15">
         <v>14</v>
@@ -7957,16 +7957,16 @@
         <v>0.03622936028224144</v>
       </c>
       <c r="I16">
-        <v>-1.291551810994642</v>
+        <v>-1.291303164203968</v>
       </c>
       <c r="J16">
-        <v>-1.409668342757167</v>
+        <v>-1.409511351701771</v>
       </c>
       <c r="K16">
-        <v>1.485726060448545</v>
+        <v>1.485801858507458</v>
       </c>
       <c r="L16">
-        <v>1.459942181423256</v>
+        <v>1.459900104530916</v>
       </c>
       <c r="M16">
         <v>-2</v>
@@ -8002,13 +8002,13 @@
         <v>37</v>
       </c>
       <c r="X16">
-        <v>0.1757187700557087</v>
+        <v>0.1757696069293094</v>
       </c>
       <c r="Y16">
         <v>-2</v>
       </c>
       <c r="Z16">
-        <v>-0.3242812299442913</v>
+        <v>-0.3242303930706905</v>
       </c>
       <c r="AA16">
         <v>15</v>
@@ -8040,16 +8040,16 @@
         <v>0.004156999999999966</v>
       </c>
       <c r="I17">
-        <v>1.026122992603929</v>
+        <v>1.02629103069344</v>
       </c>
       <c r="J17">
-        <v>0.1385107140239271</v>
+        <v>0.1385247326455501</v>
       </c>
       <c r="K17">
-        <v>-0.5032653221208153</v>
+        <v>-0.5032112154861893</v>
       </c>
       <c r="L17">
-        <v>-0.886671643749397</v>
+        <v>-0.8866003569389371</v>
       </c>
       <c r="M17">
         <v>3</v>
@@ -8085,13 +8085,13 @@
         <v>36</v>
       </c>
       <c r="X17">
-        <v>-0.2029316253574076</v>
+        <v>-0.2028629038008068</v>
       </c>
       <c r="Y17">
         <v>-0.4999999999999998</v>
       </c>
       <c r="Z17">
-        <v>-0.3279316253574075</v>
+        <v>-0.3278629038008067</v>
       </c>
       <c r="AA17">
         <v>16</v>
@@ -8123,16 +8123,16 @@
         <v>0.008294000000000024</v>
       </c>
       <c r="I18">
-        <v>0.2152627852971158</v>
+        <v>0.2154590250946633</v>
       </c>
       <c r="J18">
-        <v>1.012153076628026</v>
+        <v>1.012086415450836</v>
       </c>
       <c r="K18">
-        <v>-0.7361812230312892</v>
+        <v>-0.7361296565170851</v>
       </c>
       <c r="L18">
-        <v>-0.5839829326814215</v>
+        <v>-0.5839262686063749</v>
       </c>
       <c r="M18">
         <v>2</v>
@@ -8168,13 +8168,13 @@
         <v>37</v>
       </c>
       <c r="X18">
-        <v>-0.2304906461266385</v>
+        <v>-0.230446218798042</v>
       </c>
       <c r="Y18">
         <v>-0.5999999999999999</v>
       </c>
       <c r="Z18">
-        <v>-0.3804906461266385</v>
+        <v>-0.380446218798042</v>
       </c>
       <c r="AA18">
         <v>17</v>
@@ -8206,16 +8206,16 @@
         <v>0.02349157088044751</v>
       </c>
       <c r="I19">
-        <v>-1.127749899769848</v>
+        <v>-1.127506950007632</v>
       </c>
       <c r="J19">
-        <v>-0.6991714993395353</v>
+        <v>-0.6990801217946998</v>
       </c>
       <c r="K19">
-        <v>1.111208781579382</v>
+        <v>1.111280495249961</v>
       </c>
       <c r="L19">
-        <v>0.5279660982991882</v>
+        <v>0.5279690446904284</v>
       </c>
       <c r="M19">
         <v>-2</v>
@@ -8251,13 +8251,13 @@
         <v>37</v>
       </c>
       <c r="X19">
-        <v>0.06300213126652165</v>
+        <v>0.0630498894343437</v>
       </c>
       <c r="Y19">
         <v>-2</v>
       </c>
       <c r="Z19">
-        <v>-0.4369978687334783</v>
+        <v>-0.4369501105656562</v>
       </c>
       <c r="AA19">
         <v>18</v>
@@ -8289,16 +8289,16 @@
         <v>0.005554000000000059</v>
       </c>
       <c r="I20">
-        <v>0.3921036546293556</v>
+        <v>0.3922937439036429</v>
       </c>
       <c r="J20">
-        <v>0.4042372905178948</v>
+        <v>0.404226769616655</v>
       </c>
       <c r="K20">
-        <v>-0.6054050543983434</v>
+        <v>-0.6053520616731535</v>
       </c>
       <c r="L20">
-        <v>-0.7844584145103387</v>
+        <v>-0.7843920655682309</v>
       </c>
       <c r="M20">
         <v>2</v>
@@ -8334,13 +8334,13 @@
         <v>38</v>
       </c>
       <c r="X20">
-        <v>-0.2878988819948867</v>
+        <v>-0.2878371307850758</v>
       </c>
       <c r="Y20">
         <v>-0.5999999999999999</v>
       </c>
       <c r="Z20">
-        <v>-0.4378988819948866</v>
+        <v>-0.4378371307850757</v>
       </c>
       <c r="AA20">
         <v>19</v>
@@ -8372,16 +8372,16 @@
         <v>0.01051945602075555</v>
       </c>
       <c r="I21">
-        <v>-0.06833455353984018</v>
+        <v>-0.06812845023033598</v>
       </c>
       <c r="J21">
-        <v>0.4401974397585315</v>
+        <v>0.4401835979816907</v>
       </c>
       <c r="K21">
-        <v>-0.6662738219445684</v>
+        <v>-0.6662214930383745</v>
       </c>
       <c r="L21">
-        <v>-0.4211546961668106</v>
+        <v>-0.4211058982398339</v>
       </c>
       <c r="M21">
         <v>-1</v>
@@ -8417,13 +8417,13 @@
         <v>37</v>
       </c>
       <c r="X21">
-        <v>-0.2327823386510476</v>
+        <v>-0.232736268279459</v>
       </c>
       <c r="Y21">
         <v>-0.8999999999999998</v>
       </c>
       <c r="Z21">
-        <v>-0.4577823386510476</v>
+        <v>-0.457736268279459</v>
       </c>
       <c r="AA21">
         <v>20</v>
@@ -8455,16 +8455,16 @@
         <v>0.01108500000000001</v>
       </c>
       <c r="I22">
-        <v>0.2682335526086162</v>
+        <v>0.2684279500835282</v>
       </c>
       <c r="J22">
-        <v>0.05674869048732174</v>
+        <v>0.05677025973136399</v>
       </c>
       <c r="K22">
-        <v>-0.5603516382430519</v>
+        <v>-0.5602981541769875</v>
       </c>
       <c r="L22">
-        <v>-0.3797759729060519</v>
+        <v>-0.3797291739638402</v>
       </c>
       <c r="M22">
         <v>2</v>
@@ -8500,13 +8500,13 @@
         <v>37</v>
       </c>
       <c r="X22">
-        <v>-0.2818427872770104</v>
+        <v>-0.2817842688840067</v>
       </c>
       <c r="Y22">
         <v>-0.7999999999999998</v>
       </c>
       <c r="Z22">
-        <v>-0.4818427872770104</v>
+        <v>-0.4817842688840067</v>
       </c>
       <c r="AA22">
         <v>21</v>
@@ -8538,16 +8538,16 @@
         <v>0.0236741619528269</v>
       </c>
       <c r="I23">
-        <v>-0.8620811283306308</v>
+        <v>-0.861847418525018</v>
       </c>
       <c r="J23">
-        <v>-0.5958333862585479</v>
+        <v>-0.5957515518614923</v>
       </c>
       <c r="K23">
-        <v>0.4196250008701242</v>
+        <v>0.4196891723073138</v>
       </c>
       <c r="L23">
-        <v>0.5413255994717858</v>
+        <v>0.5413279004724192</v>
       </c>
       <c r="M23">
         <v>-2</v>
@@ -8583,13 +8583,13 @@
         <v>37</v>
       </c>
       <c r="X23">
-        <v>6.44758533165507E-05</v>
+        <v>0.0001085406683122847</v>
       </c>
       <c r="Y23">
         <v>-2</v>
       </c>
       <c r="Z23">
-        <v>-0.4999355241466834</v>
+        <v>-0.4998914593316877</v>
       </c>
       <c r="AA23">
         <v>22</v>
@@ -8621,16 +8621,16 @@
         <v>0.002985254784476865</v>
       </c>
       <c r="I24">
-        <v>-0.722727263557299</v>
+        <v>-0.7224984004773891</v>
       </c>
       <c r="J24">
-        <v>0.8039627389190772</v>
+        <v>0.8039153038637875</v>
       </c>
       <c r="K24">
-        <v>-0.7494815195346708</v>
+        <v>-0.7494300980700517</v>
       </c>
       <c r="L24">
-        <v>-0.9724038286628003</v>
+        <v>-0.972328400174734</v>
       </c>
       <c r="M24">
         <v>-2</v>
@@ -8666,13 +8666,13 @@
         <v>37</v>
       </c>
       <c r="X24">
-        <v>-0.2601803069995213</v>
+        <v>-0.26014240206166</v>
       </c>
       <c r="Y24">
         <v>-0.9999999999999998</v>
       </c>
       <c r="Z24">
-        <v>-0.5101803069995212</v>
+        <v>-0.5101424020616599</v>
       </c>
       <c r="AA24">
         <v>23</v>
@@ -8704,16 +8704,16 @@
         <v>0.007756000000000096</v>
       </c>
       <c r="I25">
-        <v>0.5518308914455723</v>
+        <v>0.5520154254085275</v>
       </c>
       <c r="J25">
-        <v>-0.07800723719337993</v>
+        <v>-0.07797322340497996</v>
       </c>
       <c r="K25">
-        <v>-0.8502605769814321</v>
+        <v>-0.8502102545870821</v>
       </c>
       <c r="L25">
-        <v>-0.6233463667047588</v>
+        <v>-0.6232878010025301</v>
       </c>
       <c r="M25">
         <v>2</v>
@@ -8749,13 +8749,13 @@
         <v>38</v>
       </c>
       <c r="X25">
-        <v>-0.3869378541529166</v>
+        <v>-0.3868696886135535</v>
       </c>
       <c r="Y25">
         <v>-0.7999999999999998</v>
       </c>
       <c r="Z25">
-        <v>-0.5869378541529165</v>
+        <v>-0.5868696886135535</v>
       </c>
       <c r="AA25">
         <v>24</v>
@@ -8787,16 +8787,16 @@
         <v>0.005562999999999985</v>
       </c>
       <c r="I26">
-        <v>-0.006399502529470485</v>
+        <v>-0.006195553320278658</v>
       </c>
       <c r="J26">
-        <v>0.2463911617458371</v>
+        <v>0.2463952177406568</v>
       </c>
       <c r="K26">
-        <v>-0.6386121271753298</v>
+        <v>-0.6385594965978653</v>
       </c>
       <c r="L26">
-        <v>-0.783799918402147</v>
+        <v>-0.7837336012716464</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -8832,13 +8832,13 @@
         <v>37</v>
       </c>
       <c r="X26">
-        <v>-0.4245127507780308</v>
+        <v>-0.4244536751828806</v>
       </c>
       <c r="Y26">
         <v>-0.7999999999999998</v>
       </c>
       <c r="Z26">
-        <v>-0.6245127507780308</v>
+        <v>-0.6244536751828806</v>
       </c>
       <c r="AA26">
         <v>25</v>
@@ -8870,16 +8870,16 @@
         <v>0.01152400000000009</v>
       </c>
       <c r="I27">
-        <v>-0.008029372292901271</v>
+        <v>-0.007825366396859119</v>
       </c>
       <c r="J27">
-        <v>-0.3952136062844697</v>
+        <v>-0.3951502988776096</v>
       </c>
       <c r="K27">
-        <v>-0.8964333326685434</v>
+        <v>-0.8963835138222948</v>
       </c>
       <c r="L27">
-        <v>-0.3476559960728726</v>
+        <v>-0.3476107488301645</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -8915,13 +8915,13 @@
         <v>37</v>
       </c>
       <c r="X27">
-        <v>-0.4536893927457834</v>
+        <v>-0.4536279135873847</v>
       </c>
       <c r="Y27">
         <v>-1.2</v>
       </c>
       <c r="Z27">
-        <v>-0.7536893927457834</v>
+        <v>-0.7536279135873847</v>
       </c>
       <c r="AA27">
         <v>26</v>
@@ -8953,16 +8953,16 @@
         <v>0.004607999999999945</v>
       </c>
       <c r="I28">
-        <v>0.4222562452528251</v>
+        <v>0.4224452858203812</v>
       </c>
       <c r="J28">
-        <v>-0.2468306746810004</v>
+        <v>-0.246781070255568</v>
       </c>
       <c r="K28">
-        <v>-0.5601650816544118</v>
+        <v>-0.5601115955538095</v>
       </c>
       <c r="L28">
-        <v>-0.8536736721052953</v>
+        <v>-0.8536039794098153</v>
       </c>
       <c r="M28">
         <v>2</v>
@@ -8998,13 +8998,13 @@
         <v>37</v>
       </c>
       <c r="X28">
-        <v>-0.5166595037493592</v>
+        <v>-0.5165867558991445</v>
       </c>
       <c r="Y28">
         <v>-1</v>
       </c>
       <c r="Z28">
-        <v>-0.7666595037493592</v>
+        <v>-0.7665867558991445</v>
       </c>
       <c r="AA28">
         <v>27</v>
@@ -9036,16 +9036,16 @@
         <v>0.01593287195180237</v>
       </c>
       <c r="I29">
-        <v>-1.012844081447978</v>
+        <v>-1.01260512810871</v>
       </c>
       <c r="J29">
-        <v>-1.364623524234685</v>
+        <v>-1.364470693012937</v>
       </c>
       <c r="K29">
-        <v>0.1736154893923004</v>
+        <v>0.1736769779135464</v>
       </c>
       <c r="L29">
-        <v>-0.02507543809492618</v>
+        <v>-0.02504577455248921</v>
       </c>
       <c r="M29">
         <v>-2</v>
@@ -9081,13 +9081,13 @@
         <v>37</v>
       </c>
       <c r="X29">
-        <v>-0.2966299655373176</v>
+        <v>-0.2965682140893749</v>
       </c>
       <c r="Y29">
         <v>-2</v>
       </c>
       <c r="Z29">
-        <v>-0.7966299655373175</v>
+        <v>-0.7965682140893748</v>
       </c>
       <c r="AA29">
         <v>28</v>
@@ -9119,16 +9119,16 @@
         <v>0.003329317480264216</v>
       </c>
       <c r="I30">
-        <v>-0.2215423113023336</v>
+        <v>-0.2213308794288988</v>
       </c>
       <c r="J30">
-        <v>-0.3728804609666005</v>
+        <v>-0.3728192159982717</v>
       </c>
       <c r="K30">
-        <v>-1.09347122204017</v>
+        <v>-1.093423552038053</v>
       </c>
       <c r="L30">
-        <v>-0.9472300568681558</v>
+        <v>-0.9471558445120125</v>
       </c>
       <c r="M30">
         <v>-2</v>
@@ -9164,13 +9164,13 @@
         <v>37</v>
       </c>
       <c r="X30">
-        <v>-0.4844280319534016</v>
+        <v>-0.4843724330688174</v>
       </c>
       <c r="Y30">
         <v>-1.4</v>
       </c>
       <c r="Z30">
-        <v>-0.8344280319534016</v>
+        <v>-0.8343724330688174</v>
       </c>
       <c r="AA30">
         <v>29</v>
@@ -9202,16 +9202,16 @@
         <v>0.01511745039651724</v>
       </c>
       <c r="I31">
-        <v>-0.6999090868692681</v>
+        <v>-0.6996810174052627</v>
       </c>
       <c r="J31">
-        <v>-1.29459586518713</v>
+        <v>-1.294449500933657</v>
       </c>
       <c r="K31">
-        <v>-0.2822241089360907</v>
+        <v>-0.2821675916833081</v>
       </c>
       <c r="L31">
-        <v>-0.08473676261663217</v>
+        <v>-0.08470421686639895</v>
       </c>
       <c r="M31">
         <v>-2</v>
@@ -9247,13 +9247,13 @@
         <v>37</v>
       </c>
       <c r="X31">
-        <v>-0.3400401577067147</v>
+        <v>-0.3399806034064606</v>
       </c>
       <c r="Y31">
         <v>-2</v>
       </c>
       <c r="Z31">
-        <v>-0.8400401577067147</v>
+        <v>-0.8399806034064605</v>
       </c>
       <c r="AA31">
         <v>30</v>
@@ -9285,16 +9285,16 @@
         <v>0.01294211206956963</v>
       </c>
       <c r="I32">
-        <v>-0.7137629798584295</v>
+        <v>-0.7135344285561964</v>
       </c>
       <c r="J32">
-        <v>-1.137506792188559</v>
+        <v>-1.137374934917976</v>
       </c>
       <c r="K32">
-        <v>-0.2993245597098933</v>
+        <v>-0.2992682289501928</v>
       </c>
       <c r="L32">
-        <v>-0.2438980762063175</v>
+        <v>-0.2438578414551684</v>
       </c>
       <c r="M32">
         <v>-2</v>
@@ -9330,13 +9330,13 @@
         <v>37</v>
       </c>
       <c r="X32">
-        <v>-0.349597873141724</v>
+        <v>-0.3495392040495664</v>
       </c>
       <c r="Y32">
         <v>-2</v>
       </c>
       <c r="Z32">
-        <v>-0.849597873141724</v>
+        <v>-0.8495392040495664</v>
       </c>
       <c r="AA32">
         <v>31</v>
@@ -9368,16 +9368,16 @@
         <v>0.01253918379911845</v>
       </c>
       <c r="I33">
-        <v>-0.6681266264823679</v>
+        <v>-0.6678996624119439</v>
       </c>
       <c r="J33">
-        <v>-0.8066734191747018</v>
+        <v>-0.8065721139596482</v>
       </c>
       <c r="K33">
-        <v>-0.7232166941190961</v>
+        <v>-0.7231649862171012</v>
       </c>
       <c r="L33">
-        <v>-0.2733788204257316</v>
+        <v>-0.2733371614750444</v>
       </c>
       <c r="M33">
         <v>-2</v>
@@ -9413,13 +9413,13 @@
         <v>37</v>
       </c>
       <c r="X33">
-        <v>-0.3603466780777715</v>
+        <v>-0.360293754510281</v>
       </c>
       <c r="Y33">
         <v>-2</v>
       </c>
       <c r="Z33">
-        <v>-0.8603466780777715</v>
+        <v>-0.8602937545102809</v>
       </c>
       <c r="AA33">
         <v>32</v>
@@ -9430,37 +9430,37 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.0083</v>
+        <v>0.0072</v>
       </c>
       <c r="C34">
-        <v>-0.3807</v>
+        <v>-0.3814</v>
       </c>
       <c r="D34">
-        <v>0.013811</v>
+        <v>0.013784</v>
       </c>
       <c r="E34">
-        <v>0.011368</v>
+        <v>0.011344</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34">
-        <v>0.01381100000000002</v>
+        <v>0.01378400000000002</v>
       </c>
       <c r="H34">
-        <v>0.01136800000000004</v>
+        <v>0.01134400000000002</v>
       </c>
       <c r="I34">
-        <v>0.009084260223121938</v>
+        <v>0.0003236989860431619</v>
       </c>
       <c r="J34">
-        <v>-2.081176813840214</v>
+        <v>-2.083607260313649</v>
       </c>
       <c r="K34">
-        <v>0.04203958645853996</v>
+        <v>0.03958109863427624</v>
       </c>
       <c r="L34">
-        <v>-0.3590699286149603</v>
+        <v>-0.3607800347619704</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -9496,13 +9496,13 @@
         <v>37</v>
       </c>
       <c r="X34">
-        <v>-0.508099019996362</v>
+        <v>-0.5106878928251266</v>
       </c>
       <c r="Y34">
         <v>-1.8</v>
       </c>
       <c r="Z34">
-        <v>-0.9580990199963619</v>
+        <v>-0.9606878928251266</v>
       </c>
       <c r="AA34">
         <v>33</v>
@@ -9534,16 +9534,16 @@
         <v>0.009338999999999986</v>
       </c>
       <c r="I35">
-        <v>0.04657126478202991</v>
+        <v>0.04677337166858616</v>
       </c>
       <c r="J35">
-        <v>-0.7597359612185023</v>
+        <v>-0.7596389906200229</v>
       </c>
       <c r="K35">
-        <v>-0.8285267344054913</v>
+        <v>-0.8284761749874896</v>
       </c>
       <c r="L35">
-        <v>-0.5075242178963071</v>
+        <v>-0.5074712475023111</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -9579,13 +9579,13 @@
         <v>37</v>
       </c>
       <c r="X35">
-        <v>-0.5569377291184711</v>
+        <v>-0.5568670855825151</v>
       </c>
       <c r="Y35">
         <v>-1.7</v>
       </c>
       <c r="Z35">
-        <v>-0.981937729118471</v>
+        <v>-0.981867085582515</v>
       </c>
       <c r="AA35">
         <v>34</v>
@@ -9617,16 +9617,16 @@
         <v>0.006153999999999993</v>
       </c>
       <c r="I36">
-        <v>0.005009585814544994</v>
+        <v>0.005213138215784543</v>
       </c>
       <c r="J36">
-        <v>-0.5507885677360661</v>
+        <v>-0.5507108931726582</v>
       </c>
       <c r="K36">
-        <v>-0.8067928918295504</v>
+        <v>-0.8067420953878971</v>
       </c>
       <c r="L36">
-        <v>-0.7405586739638648</v>
+        <v>-0.740494445795566</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -9662,13 +9662,13 @@
         <v>37</v>
       </c>
       <c r="X36">
-        <v>-0.6025638256531579</v>
+        <v>-0.6024923827252203</v>
       </c>
       <c r="Y36">
         <v>-1.6</v>
       </c>
       <c r="Z36">
-        <v>-1.002563825653158</v>
+        <v>-1.00249238272522</v>
       </c>
       <c r="AA36">
         <v>35</v>
@@ -9700,16 +9700,16 @@
         <v>0.002719829125617412</v>
       </c>
       <c r="I37">
-        <v>-0.1058215580987482</v>
+        <v>-0.1056141509916865</v>
       </c>
       <c r="J37">
-        <v>-0.7847188017435761</v>
+        <v>-0.7846195240104687</v>
       </c>
       <c r="K37">
-        <v>-1.069856229596596</v>
+        <v>-1.069808302055494</v>
       </c>
       <c r="L37">
-        <v>-0.991824024593314</v>
+        <v>-0.991747657925605</v>
       </c>
       <c r="M37">
         <v>-1</v>
@@ -9745,13 +9745,13 @@
         <v>37</v>
       </c>
       <c r="X37">
-        <v>-0.6914271849527744</v>
+        <v>-0.6913583105630441</v>
       </c>
       <c r="Y37">
         <v>-1.9</v>
       </c>
       <c r="Z37">
-        <v>-1.166427184952775</v>
+        <v>-1.166358310563044</v>
       </c>
       <c r="AA37">
         <v>36</v>

</xml_diff>